<commit_message>
making limit later, interpolate with polyfit,
</commit_message>
<xml_diff>
--- a/data/Traderes_data.xlsx
+++ b/data/Traderes_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE381EC-AF62-443D-9B93-7DA985517247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5877BBAB-27AF-489F-A13F-6F49FEABDA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3680" yWindow="-16810" windowWidth="21600" windowHeight="12740" tabRatio="785" activeTab="5" xr2:uid="{9A6D5CBA-73A9-44EC-81CD-5563DD7C030A}"/>
+    <workbookView xWindow="6375" yWindow="3015" windowWidth="21600" windowHeight="12735" tabRatio="785" activeTab="5" xr2:uid="{9A6D5CBA-73A9-44EC-81CD-5563DD7C030A}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="12" r:id="rId1"/>
@@ -3390,7 +3390,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,7 +3430,10 @@
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <f>C2</f>
+        <v>26.81</v>
+      </c>
       <c r="C2" s="28">
         <v>26.81</v>
       </c>
@@ -3440,7 +3443,10 @@
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <f t="shared" ref="B3:B7" si="0">C3</f>
+        <v>8.93</v>
+      </c>
       <c r="C3" s="28">
         <v>8.93</v>
       </c>
@@ -3450,7 +3456,10 @@
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <f t="shared" si="0"/>
+        <v>6.48</v>
+      </c>
       <c r="C4" s="28">
         <v>6.48</v>
       </c>
@@ -3460,7 +3469,10 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.69</v>
+      </c>
       <c r="C5" s="28">
         <v>1.69</v>
       </c>
@@ -3472,7 +3484,10 @@
       <c r="A6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>40.68</v>
+      </c>
       <c r="C6" s="28">
         <v>40.68</v>
       </c>

</xml_diff>